<commit_message>
add year and month
</commit_message>
<xml_diff>
--- a/public/cambodia_export.xlsx
+++ b/public/cambodia_export.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leangchanmolika/Desktop/software_access_managements/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A827F86C-898D-B74B-96B1-4B9FE59BF1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88EC5C6-18BA-F74F-BBF0-3A469A2404FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{C72DAF18-C3B1-0446-810C-E71F3B8E8823}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -295,16 +295,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC3956E-4CCE-1E43-A32A-3A7CB38FC227}">
   <dimension ref="A1:V200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I102" sqref="I102"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,6 +840,7 @@
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="55.5" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
@@ -1099,83 +1100,83 @@
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="10" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="10" t="s">
+      <c r="J11" s="11"/>
+      <c r="K11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="N11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O11" s="13"/>
-      <c r="P11" s="12" t="s">
+      <c r="O11" s="11"/>
+      <c r="P11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="12" t="s">
+      <c r="Q11" s="11"/>
+      <c r="R11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="S11" s="13"/>
-      <c r="T11" s="10" t="s">
+      <c r="S11" s="11"/>
+      <c r="T11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="U11" s="10" t="s">
+      <c r="U11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" ht="26" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1194,8 +1195,8 @@
       <c r="S12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" ht="26" x14ac:dyDescent="0.55000000000000004">
@@ -1203,7 +1204,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="H13" s="6"/>
@@ -1227,7 +1228,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="6"/>
@@ -1251,7 +1252,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
       <c r="H15" s="6"/>
@@ -1275,7 +1276,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
       <c r="H16" s="6"/>
@@ -1299,7 +1300,7 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="6"/>
@@ -1323,7 +1324,7 @@
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
       <c r="H18" s="6"/>
@@ -1347,7 +1348,7 @@
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
       <c r="H19" s="6"/>
@@ -1371,7 +1372,7 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
       <c r="H20" s="6"/>
@@ -1395,7 +1396,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
       <c r="H21" s="6"/>
@@ -1419,7 +1420,7 @@
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
       <c r="H22" s="6"/>
@@ -1443,7 +1444,7 @@
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
       <c r="H23" s="6"/>
@@ -1467,7 +1468,7 @@
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
       <c r="H24" s="6"/>
@@ -1491,7 +1492,7 @@
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
       <c r="H25" s="6"/>
@@ -1515,7 +1516,7 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
       <c r="H26" s="6"/>
@@ -1539,7 +1540,7 @@
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
       <c r="H27" s="6"/>
@@ -1563,7 +1564,7 @@
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
       <c r="H28" s="6"/>
@@ -1587,7 +1588,7 @@
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
       <c r="H29" s="6"/>
@@ -1611,7 +1612,7 @@
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
       <c r="H30" s="6"/>
@@ -1635,7 +1636,7 @@
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
+      <c r="E31" s="6"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
       <c r="H31" s="6"/>
@@ -1659,7 +1660,7 @@
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="6"/>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
       <c r="H32" s="6"/>
@@ -1683,7 +1684,7 @@
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
+      <c r="E33" s="6"/>
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
       <c r="H33" s="6"/>
@@ -1707,7 +1708,7 @@
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
+      <c r="E34" s="6"/>
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
       <c r="H34" s="6"/>
@@ -1731,7 +1732,7 @@
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
       <c r="H35" s="6"/>
@@ -1755,7 +1756,7 @@
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
       <c r="H36" s="6"/>
@@ -1779,7 +1780,7 @@
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
+      <c r="E37" s="6"/>
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
       <c r="H37" s="6"/>
@@ -1803,7 +1804,7 @@
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
       <c r="H38" s="6"/>
@@ -1827,7 +1828,7 @@
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
+      <c r="E39" s="6"/>
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
       <c r="H39" s="6"/>
@@ -1851,7 +1852,7 @@
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="7"/>
+      <c r="E40" s="6"/>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
       <c r="H40" s="6"/>
@@ -1875,7 +1876,7 @@
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="6"/>
@@ -1899,7 +1900,7 @@
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
+      <c r="E42" s="6"/>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="6"/>
@@ -1923,7 +1924,7 @@
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
       <c r="H43" s="6"/>
@@ -1947,7 +1948,7 @@
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
+      <c r="E44" s="6"/>
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
       <c r="H44" s="6"/>
@@ -1971,7 +1972,7 @@
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
+      <c r="E45" s="6"/>
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
       <c r="H45" s="6"/>
@@ -1995,7 +1996,7 @@
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="7"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
       <c r="H46" s="6"/>
@@ -2019,7 +2020,7 @@
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
       <c r="H47" s="6"/>
@@ -2043,7 +2044,7 @@
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
       <c r="H48" s="6"/>
@@ -2067,7 +2068,7 @@
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="7"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
       <c r="H49" s="6"/>
@@ -2091,7 +2092,7 @@
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="7"/>
+      <c r="E50" s="6"/>
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
       <c r="H50" s="6"/>
@@ -2114,7 +2115,7 @@
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="6"/>
-      <c r="E51" s="7"/>
+      <c r="E51" s="6"/>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
       <c r="H51" s="6"/>
@@ -2137,7 +2138,7 @@
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="7"/>
+      <c r="E52" s="6"/>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
       <c r="H52" s="6"/>
@@ -2160,7 +2161,7 @@
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="7"/>
+      <c r="E53" s="6"/>
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
       <c r="H53" s="6"/>
@@ -2183,7 +2184,7 @@
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="6"/>
-      <c r="E54" s="7"/>
+      <c r="E54" s="6"/>
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
       <c r="H54" s="6"/>
@@ -2206,7 +2207,7 @@
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="6"/>
-      <c r="E55" s="7"/>
+      <c r="E55" s="6"/>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
       <c r="H55" s="6"/>
@@ -2229,7 +2230,7 @@
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="6"/>
-      <c r="E56" s="7"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
       <c r="H56" s="6"/>
@@ -2252,7 +2253,7 @@
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
       <c r="D57" s="6"/>
-      <c r="E57" s="7"/>
+      <c r="E57" s="6"/>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
       <c r="H57" s="6"/>
@@ -2275,7 +2276,7 @@
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
       <c r="D58" s="6"/>
-      <c r="E58" s="7"/>
+      <c r="E58" s="6"/>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
       <c r="H58" s="6"/>
@@ -2298,7 +2299,7 @@
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="6"/>
-      <c r="E59" s="7"/>
+      <c r="E59" s="6"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
       <c r="H59" s="6"/>
@@ -2321,7 +2322,7 @@
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="7"/>
+      <c r="E60" s="6"/>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
       <c r="H60" s="6"/>
@@ -2344,7 +2345,7 @@
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="7"/>
+      <c r="E61" s="6"/>
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
       <c r="H61" s="6"/>
@@ -2367,7 +2368,7 @@
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="6"/>
-      <c r="E62" s="7"/>
+      <c r="E62" s="6"/>
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
       <c r="H62" s="6"/>
@@ -2390,7 +2391,7 @@
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
       <c r="D63" s="6"/>
-      <c r="E63" s="7"/>
+      <c r="E63" s="6"/>
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
       <c r="H63" s="6"/>
@@ -2413,7 +2414,7 @@
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
       <c r="D64" s="6"/>
-      <c r="E64" s="7"/>
+      <c r="E64" s="6"/>
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
       <c r="H64" s="6"/>
@@ -2436,7 +2437,7 @@
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="6"/>
-      <c r="E65" s="7"/>
+      <c r="E65" s="6"/>
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
       <c r="H65" s="6"/>
@@ -2459,7 +2460,7 @@
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="6"/>
-      <c r="E66" s="7"/>
+      <c r="E66" s="6"/>
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
       <c r="H66" s="6"/>
@@ -2482,7 +2483,7 @@
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
       <c r="D67" s="6"/>
-      <c r="E67" s="7"/>
+      <c r="E67" s="6"/>
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
       <c r="H67" s="6"/>
@@ -2505,7 +2506,7 @@
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
       <c r="D68" s="6"/>
-      <c r="E68" s="7"/>
+      <c r="E68" s="6"/>
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
       <c r="H68" s="6"/>
@@ -2528,7 +2529,7 @@
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
       <c r="D69" s="6"/>
-      <c r="E69" s="7"/>
+      <c r="E69" s="6"/>
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
       <c r="H69" s="6"/>
@@ -2551,7 +2552,7 @@
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
       <c r="D70" s="6"/>
-      <c r="E70" s="7"/>
+      <c r="E70" s="6"/>
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
       <c r="H70" s="6"/>
@@ -5561,6 +5562,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="P11:Q11"/>
     <mergeCell ref="R11:S11"/>
     <mergeCell ref="T11:T12"/>
@@ -5574,11 +5580,6 @@
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="35" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>